<commit_message>
Added fmul corner tests, status: 76/256 failing
</commit_message>
<xml_diff>
--- a/Project/Specifications/ISA.xlsx
+++ b/Project/Specifications/ISA.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="163">
   <si>
     <t>ECE 554 32-bit ISA
 General Format
@@ -24,11 +24,11 @@
     2 register instruction: aaaa_axxx_xxxd_dddd_xxxs_ssss_iiii_iiii
     1 register instruction: aaaa_axxx_xxxd_dddd_oooo_oooo_oooo_oooo
 a=opcode, c=sub_opcode, x=don't_care, d=destination, s=source, t=second_source, i=immediate, o=offset
-Floating Point Format:    seee_eeee_emmm_mmmm_mmmm_mmmm_mmmm_mmmm        Value = [(-1)^s] * (2^E) * (1.M), NO representation of absolute 0
+Floating Point Format:  IEEE 754: https://en.wikipedia.org/wiki/IEEE_754
 1. Flag registers are Z-zero, V-overflow, N-negative/sign
 2. The overflow flag denotes positive overflow as well as negative underflow
 3. Register R0 is hard-wired to 32'h00000000, can't be written to
-4. Jal instruction always stores the return address in register R15. Do not write R15 inside function calls if you wish to return.</t>
+4. Jal instruction always stores the return address in register R31. Do not write R31 inside function calls if you wish to return.</t>
   </si>
   <si>
     <t>Instruction</t>
@@ -430,7 +430,7 @@
     <t>MUL R1, R2, R3</t>
   </si>
   <si>
-    <t>5'b10100</t>
+    <t>5'b11000</t>
   </si>
   <si>
     <t>R1 &lt;= (signed) R2[15:0] * (signed) R3[15:0]</t>
@@ -445,7 +445,7 @@
     <t>UMUL R1, R2, R3</t>
   </si>
   <si>
-    <t>5'b10101</t>
+    <t>5'b11001</t>
   </si>
   <si>
     <t>R1 &lt;= (unsigned) R2[15:0] * (unsigned) R3[15:0]</t>
@@ -457,13 +457,13 @@
     <t>ADDF R1, R2, R3</t>
   </si>
   <si>
-    <t>5'b11000</t>
+    <t>5'b11010</t>
   </si>
   <si>
     <t>R1 &lt;= R2 + R3 (floating-point)</t>
   </si>
   <si>
-    <t>Floating point calacuation
+    <t>Floating point calculation
 1-bit sign, 8-bit exponent, 23-bit mantissa</t>
   </si>
   <si>
@@ -473,7 +473,7 @@
     <t>SUBF R1, R2, R3</t>
   </si>
   <si>
-    <t>5'b11001</t>
+    <t>5'b11011</t>
   </si>
   <si>
     <t>R1 &lt;= R2 - R3 (floating-point)</t>
@@ -485,10 +485,10 @@
     <t>MULF R1, R2, R3</t>
   </si>
   <si>
-    <t>5'b11010</t>
+    <t>5'b11100</t>
   </si>
   <si>
-    <t>R1 &lt;= R2[15:0] * R3[15:0] (floating-point)</t>
+    <t>R1 &lt;= R2* R3(floating-point)</t>
   </si>
   <si>
     <t>ITF</t>
@@ -500,7 +500,7 @@
     <t>ITF R1, R2</t>
   </si>
   <si>
-    <t>5'b11100</t>
+    <t>5'b11101</t>
   </si>
   <si>
     <t>R1 &lt;= R2 (integer to floating-point)</t>
@@ -512,7 +512,7 @@
     <t>FTI R1, R2</t>
   </si>
   <si>
-    <t>5'b11101</t>
+    <t>5'b11110</t>
   </si>
   <si>
     <t>R1 &lt;= R2 (floating-point to integer)</t>
@@ -2224,24 +2224,12 @@
       <c r="Z36" s="20"/>
     </row>
     <row r="37">
-      <c r="A37" s="19" t="s">
-        <v>128</v>
-      </c>
-      <c r="B37" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="C37" s="19" t="s">
-        <v>129</v>
-      </c>
-      <c r="D37" s="19" t="s">
-        <v>130</v>
-      </c>
-      <c r="E37" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="F37" s="21" t="s">
-        <v>132</v>
-      </c>
+      <c r="A37" s="14"/>
+      <c r="B37" s="14"/>
+      <c r="C37" s="14"/>
+      <c r="D37" s="14"/>
+      <c r="E37" s="14"/>
+      <c r="F37" s="14"/>
       <c r="G37" s="20"/>
       <c r="H37" s="20"/>
       <c r="I37" s="20"/>
@@ -2265,19 +2253,23 @@
     </row>
     <row r="38">
       <c r="A38" s="19" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
-      <c r="B38" s="12"/>
+      <c r="B38" s="21" t="s">
+        <v>8</v>
+      </c>
       <c r="C38" s="19" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="D38" s="19" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
-      <c r="F38" s="12"/>
+      <c r="F38" s="21" t="s">
+        <v>132</v>
+      </c>
       <c r="G38" s="20"/>
       <c r="H38" s="20"/>
       <c r="I38" s="20"/>
@@ -2300,12 +2292,20 @@
       <c r="Z38" s="20"/>
     </row>
     <row r="39">
-      <c r="A39" s="14"/>
-      <c r="B39" s="14"/>
-      <c r="C39" s="14"/>
-      <c r="D39" s="14"/>
-      <c r="E39" s="14"/>
-      <c r="F39" s="14"/>
+      <c r="A39" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="B39" s="10"/>
+      <c r="C39" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="D39" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="E39" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="F39" s="12"/>
       <c r="G39" s="20"/>
       <c r="H39" s="20"/>
       <c r="I39" s="20"/>
@@ -2331,9 +2331,7 @@
       <c r="A40" s="19" t="s">
         <v>137</v>
       </c>
-      <c r="B40" s="8" t="s">
-        <v>8</v>
-      </c>
+      <c r="B40" s="10"/>
       <c r="C40" s="19" t="s">
         <v>138</v>
       </c>
@@ -29684,16 +29682,15 @@
       <c r="Z1014" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="17">
+  <mergeCells count="16">
     <mergeCell ref="B13:B14"/>
     <mergeCell ref="B16:B17"/>
     <mergeCell ref="B19:B27"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="B40:B42"/>
+    <mergeCell ref="B38:B42"/>
     <mergeCell ref="B43:B44"/>
     <mergeCell ref="F16:F17"/>
     <mergeCell ref="F20:F27"/>
-    <mergeCell ref="F37:F38"/>
+    <mergeCell ref="F38:F39"/>
     <mergeCell ref="F40:F44"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="B3:B7"/>
@@ -29703,7 +29700,7 @@
     <mergeCell ref="F9:F11"/>
     <mergeCell ref="F13:F14"/>
   </mergeCells>
-  <conditionalFormatting sqref="A1:F28 A31:E33 F33 E37:E38 B40:B44 E40:E42">
+  <conditionalFormatting sqref="A1:F28 A31:E33 F33 E38:E42 B43:B44">
     <cfRule type="notContainsBlanks" dxfId="0" priority="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>

</xml_diff>